<commit_message>
added cinebench redshift performance data
</commit_message>
<xml_diff>
--- a/data/prods.xlsx
+++ b/data/prods.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="raster" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="rt" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="blender" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="videos" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="42">
   <si>
     <t xml:space="preserve">ProductName</t>
   </si>
@@ -99,7 +100,7 @@
     <t xml:space="preserve">Radeon Rx 7700 Xt</t>
   </si>
   <si>
-    <t xml:space="preserve">Rx 7700 Xt</t>
+    <t xml:space="preserve">Radeon Rx 7800 Xt</t>
   </si>
   <si>
     <t xml:space="preserve">Radeon Rx 7900 Xt</t>
@@ -144,7 +145,10 @@
     <t xml:space="preserve">OneAPI</t>
   </si>
   <si>
-    <t xml:space="preserve">Radeon Rx 7800 Xt</t>
+    <t xml:space="preserve">redshift_seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">redshift_score</t>
   </si>
 </sst>
 </file>
@@ -154,7 +158,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -184,6 +188,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -228,7 +239,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -239,6 +250,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -260,11 +275,11 @@
   </sheetPr>
   <dimension ref="A1:A36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.49"/>
   </cols>
@@ -389,12 +404,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>25</v>
       </c>
@@ -467,11 +482,11 @@
   </sheetPr>
   <dimension ref="A1:A36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.49"/>
   </cols>
@@ -596,12 +611,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>25</v>
       </c>
@@ -674,11 +689,11 @@
   </sheetPr>
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
@@ -923,7 +938,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B26" s="2" t="n">
         <v>2431.02</v>
@@ -1013,6 +1028,400 @@
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AMJ36"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="str">
+        <f aca="false">IFERROR(1000000/B2, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>338</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <f aca="false">IFERROR(1000000/B3, "")</f>
+        <v>2958.5798816568</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0" t="str">
+        <f aca="false">IFERROR(1000000/B4, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>266</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <f aca="false">IFERROR(1000000/B5, "")</f>
+        <v>3759.3984962406</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="0" t="str">
+        <f aca="false">IFERROR(1000000/B6, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>237</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <f aca="false">IFERROR(1000000/B7, "")</f>
+        <v>4219.40928270042</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>207</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <f aca="false">IFERROR(1000000/B8, "")</f>
+        <v>4830.91787439614</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="0" t="str">
+        <f aca="false">IFERROR(1000000/B9, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="0" t="str">
+        <f aca="false">IFERROR(1000000/B10, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="0" t="str">
+        <f aca="false">IFERROR(1000000/B11, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="0" t="str">
+        <f aca="false">IFERROR(1000000/B12, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="0" t="str">
+        <f aca="false">IFERROR(1000000/B13, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="0" t="str">
+        <f aca="false">IFERROR(1000000/B14, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="0" t="str">
+        <f aca="false">IFERROR(1000000/B15, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="0" t="str">
+        <f aca="false">IFERROR(1000000/B16, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>373</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <f aca="false">IFERROR(1000000/B17, "")</f>
+        <v>2680.96514745308</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>210</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <f aca="false">IFERROR(1000000/B18, "")</f>
+        <v>4761.90476190476</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>143</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <f aca="false">IFERROR(1000000/B19, "")</f>
+        <v>6993.00699300699</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="0" t="str">
+        <f aca="false">IFERROR(1000000/B20, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>326</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <f aca="false">IFERROR(1000000/B21, "")</f>
+        <v>3067.48466257669</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="0" t="str">
+        <f aca="false">IFERROR(1000000/B22, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="0" t="str">
+        <f aca="false">IFERROR(1000000/B23, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="0" t="str">
+        <f aca="false">IFERROR(1000000/B24, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="0" t="str">
+        <f aca="false">IFERROR(1000000/B25, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="0" t="str">
+        <f aca="false">IFERROR(1000000/B26, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="0" t="str">
+        <f aca="false">IFERROR(1000000/B27, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="0" t="str">
+        <f aca="false">IFERROR(1000000/B28, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="0" t="str">
+        <f aca="false">IFERROR(1000000/B29, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <f aca="false">IFERROR(1000000/B30, "")</f>
+        <v>9345.79439252336</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <f aca="false">IFERROR(1000000/B31, "")</f>
+        <v>13157.8947368421</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>162</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <f aca="false">IFERROR(1000000/B32, "")</f>
+        <v>6172.83950617284</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>156</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <f aca="false">IFERROR(1000000/B33, "")</f>
+        <v>6410.25641025641</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="0" t="str">
+        <f aca="false">IFERROR(1000000/B34, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="0" t="str">
+        <f aca="false">IFERROR(1000000/B35, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="0" t="str">
+        <f aca="false">IFERROR(1000000/B36, "")</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>